<commit_message>
incluido trilha de cursos do bb
</commit_message>
<xml_diff>
--- a/Trilha Transformação Digital 2019-1.xlsx
+++ b/Trilha Transformação Digital 2019-1.xlsx
@@ -588,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,22 +703,22 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="5">
         <v>5426</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="4" t="s">
+      <c r="C6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
atualizado a lista de cursos bb
</commit_message>
<xml_diff>
--- a/Trilha Transformação Digital 2019-1.xlsx
+++ b/Trilha Transformação Digital 2019-1.xlsx
@@ -13,17 +13,17 @@
   <calcPr iterateDelta="0.0001"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1550531027" val="944" rev="123" revOS="3"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1550531027" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1550531027" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1550531027"/>
+      <pm:revision xmlns:pm="smNativeData" day="1550624566" val="944" rev="123" revOS="3"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1550624566" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1550624566" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1550624566"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="56">
   <si>
     <t>codigo do curso</t>
   </si>
@@ -220,7 +220,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1550531027" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1550624566" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -235,7 +235,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1550531027" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1550624566" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -250,7 +250,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1550531027" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1550624566" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -266,7 +266,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1550531027" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1550624566" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default" weight="bold"/>
             <pm:cs face="Basic Roman" sz="220" lang="default" weight="bold"/>
             <pm:ea face="Basic Roman" sz="220" lang="default" weight="bold"/>
@@ -288,7 +288,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1550531027" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1550624566" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -299,7 +299,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1550531027" type="1" fgLvl="100" fgClr="00C0C0C0" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1550624566" type="1" fgLvl="100" fgClr="00C0C0C0" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -310,7 +310,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1550531027" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1550624566" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -324,7 +324,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1550531027" type="1" fgLvl="100" fgClr="00BDD7EE" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1550624566" type="1" fgLvl="100" fgClr="00BDD7EE" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -335,7 +335,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1550531027" type="1" fgLvl="100" fgClr="0099CCFF" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1550624566" type="1" fgLvl="100" fgClr="0099CCFF" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -346,7 +346,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1550531027" type="1" fgLvl="100" fgClr="00B8CCE4" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1550624566" type="1" fgLvl="100" fgClr="00B8CCE4" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -357,7 +357,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1550531027" type="1" fgLvl="100" fgClr="00B8CCE4" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1550624566" type="1" fgLvl="100" fgClr="00B8CCE4" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -368,7 +368,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1550531027" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1550624566" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -390,7 +390,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1550531027"/>
+          <pm:border xmlns:pm="smNativeData" id="1550624566"/>
         </ext>
       </extLst>
     </border>
@@ -409,7 +409,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1550531027"/>
+          <pm:border xmlns:pm="smNativeData" id="1550624566"/>
         </ext>
       </extLst>
     </border>
@@ -428,7 +428,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1550531027">
+          <pm:border xmlns:pm="smNativeData" id="1550624566">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -452,7 +452,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1550531027">
+          <pm:border xmlns:pm="smNativeData" id="1550624566">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -476,7 +476,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1550531027">
+          <pm:border xmlns:pm="smNativeData" id="1550624566">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -500,7 +500,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1550531027">
+          <pm:border xmlns:pm="smNativeData" id="1550624566">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -524,7 +524,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1550531027">
+          <pm:border xmlns:pm="smNativeData" id="1550624566">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -548,7 +548,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1550531027">
+          <pm:border xmlns:pm="smNativeData" id="1550624566">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -572,7 +572,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1550531027">
+          <pm:border xmlns:pm="smNativeData" id="1550624566">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -596,7 +596,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1550531027"/>
+          <pm:border xmlns:pm="smNativeData" id="1550624566"/>
         </ext>
       </extLst>
     </border>
@@ -653,10 +653,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1550531027" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1550624566" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1550531027" count="3">
+      <pm:colors xmlns:pm="smNativeData" id="1550624566" count="3">
         <pm:color name="Cor 24" rgb="BDD7EE"/>
         <pm:color name="Cor 25" rgb="99CCFF"/>
         <pm:color name="Cor 26" rgb="B8CCE4"/>
@@ -895,8 +895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" topLeftCell="C24" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" view="normal" topLeftCell="C24" zoomScale="90" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.40"/>
@@ -1535,24 +1535,27 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="9" t="n">
+    <row r="31" spans="1:7">
+      <c r="A31" s="12" t="n">
         <v>7103</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C31" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="F31" s="10" t="s">
-        <v>9</v>
+      <c r="C31" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1819,7 +1822,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1550531027" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1550624566" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1828,14 +1831,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1550531027" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1550531027" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1550624566" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1550624566" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1550531027" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1550624566" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
arquivos de configuração do projeto django
</commit_message>
<xml_diff>
--- a/Trilha Transformação Digital 2019-1.xlsx
+++ b/Trilha Transformação Digital 2019-1.xlsx
@@ -13,17 +13,17 @@
   <calcPr iterateDelta="0.0001"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1550793894" val="944" rev="123" revOS="3"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1550793894" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1550793894" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1550793894"/>
+      <pm:revision xmlns:pm="smNativeData" day="1551310064" val="944" rev="123" revOS="3"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1551310064" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1551310064" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1551310064"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="56">
   <si>
     <t>codigo do curso</t>
   </si>
@@ -220,7 +220,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1550793894" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1551310064" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -235,7 +235,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1550793894" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1551310064" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -250,7 +250,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1550793894" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1551310064" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -266,7 +266,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1550793894" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1551310064" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default" weight="bold"/>
             <pm:cs face="Basic Roman" sz="220" lang="default" weight="bold"/>
             <pm:ea face="Basic Roman" sz="220" lang="default" weight="bold"/>
@@ -288,7 +288,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1550793894" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1551310064" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -299,7 +299,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1550793894" type="1" fgLvl="100" fgClr="00C0C0C0" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1551310064" type="1" fgLvl="100" fgClr="00C0C0C0" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -310,7 +310,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1550793894" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1551310064" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -324,7 +324,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1550793894" type="1" fgLvl="100" fgClr="00BDD7EE" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1551310064" type="1" fgLvl="100" fgClr="00BDD7EE" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -335,7 +335,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1550793894" type="1" fgLvl="100" fgClr="0099CCFF" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1551310064" type="1" fgLvl="100" fgClr="0099CCFF" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -346,7 +346,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1550793894" type="1" fgLvl="100" fgClr="00B8CCE4" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1551310064" type="1" fgLvl="100" fgClr="00B8CCE4" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -357,7 +357,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1550793894" type="1" fgLvl="100" fgClr="00B8CCE4" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1551310064" type="1" fgLvl="100" fgClr="00B8CCE4" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -368,7 +368,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1550793894" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1551310064" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -390,7 +390,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1550793894"/>
+          <pm:border xmlns:pm="smNativeData" id="1551310064"/>
         </ext>
       </extLst>
     </border>
@@ -409,7 +409,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1550793894"/>
+          <pm:border xmlns:pm="smNativeData" id="1551310064"/>
         </ext>
       </extLst>
     </border>
@@ -428,7 +428,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1550793894">
+          <pm:border xmlns:pm="smNativeData" id="1551310064">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -452,7 +452,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1550793894">
+          <pm:border xmlns:pm="smNativeData" id="1551310064">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -476,7 +476,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1550793894">
+          <pm:border xmlns:pm="smNativeData" id="1551310064">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -500,7 +500,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1550793894">
+          <pm:border xmlns:pm="smNativeData" id="1551310064">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -524,7 +524,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1550793894">
+          <pm:border xmlns:pm="smNativeData" id="1551310064">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -548,7 +548,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1550793894">
+          <pm:border xmlns:pm="smNativeData" id="1551310064">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -572,7 +572,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1550793894">
+          <pm:border xmlns:pm="smNativeData" id="1551310064">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -596,7 +596,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1550793894"/>
+          <pm:border xmlns:pm="smNativeData" id="1551310064"/>
         </ext>
       </extLst>
     </border>
@@ -653,10 +653,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1550793894" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1551310064" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1550793894" count="3">
+      <pm:colors xmlns:pm="smNativeData" id="1551310064" count="3">
         <pm:color name="Cor 24" rgb="BDD7EE"/>
         <pm:color name="Cor 25" rgb="99CCFF"/>
         <pm:color name="Cor 26" rgb="B8CCE4"/>
@@ -895,8 +895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" topLeftCell="B28" zoomScale="80" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" view="normal" topLeftCell="B32" zoomScale="80" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.40"/>
@@ -1661,24 +1661,27 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="9" t="n">
+    <row r="37" spans="1:7">
+      <c r="A37" s="12" t="n">
         <v>7111</v>
       </c>
-      <c r="B37" s="10" t="s">
+      <c r="B37" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C37" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D37" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E37" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="F37" s="10" t="s">
-        <v>9</v>
+      <c r="C37" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F37" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1825,7 +1828,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1550793894" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1551310064" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1834,14 +1837,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1550793894" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1550793894" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1551310064" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1551310064" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1550793894" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1551310064" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>